<commit_message>
Added peak finding and labelling routines..
</commit_message>
<xml_diff>
--- a/User_Data/TreasuryData/TGA_Since2005.xlsx
+++ b/User_Data/TreasuryData/TGA_Since2005.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4739"/>
+  <dimension ref="A1:E4752"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -72698,6 +72698,227 @@
         <v>845541</v>
       </c>
     </row>
+    <row r="4740">
+      <c r="A4740" s="2" t="n">
+        <v>45419</v>
+      </c>
+      <c r="B4740" t="n">
+        <v>866863</v>
+      </c>
+      <c r="C4740" t="n">
+        <v>845541</v>
+      </c>
+      <c r="D4740" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4740" t="n">
+        <v>845541</v>
+      </c>
+    </row>
+    <row r="4741">
+      <c r="A4741" s="2" t="n">
+        <v>45420</v>
+      </c>
+      <c r="B4741" t="n">
+        <v>845541</v>
+      </c>
+      <c r="C4741" t="n">
+        <v>816809</v>
+      </c>
+      <c r="D4741" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4741" t="n">
+        <v>816809</v>
+      </c>
+    </row>
+    <row r="4742">
+      <c r="A4742" s="2" t="n">
+        <v>45421</v>
+      </c>
+      <c r="B4742" t="n">
+        <v>816809</v>
+      </c>
+      <c r="C4742" t="n">
+        <v>804246</v>
+      </c>
+      <c r="D4742" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4742" t="n">
+        <v>804246</v>
+      </c>
+    </row>
+    <row r="4743">
+      <c r="A4743" s="2" t="n">
+        <v>45422</v>
+      </c>
+      <c r="B4743" t="n">
+        <v>804246</v>
+      </c>
+      <c r="C4743" t="n">
+        <v>795161</v>
+      </c>
+      <c r="D4743" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4743" t="n">
+        <v>795161</v>
+      </c>
+    </row>
+    <row r="4744">
+      <c r="A4744" s="2" t="n">
+        <v>45425</v>
+      </c>
+      <c r="B4744" t="n">
+        <v>795161</v>
+      </c>
+      <c r="C4744" t="n">
+        <v>808430</v>
+      </c>
+      <c r="D4744" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4744" t="n">
+        <v>808430</v>
+      </c>
+    </row>
+    <row r="4745">
+      <c r="A4745" s="2" t="n">
+        <v>45426</v>
+      </c>
+      <c r="B4745" t="n">
+        <v>808430</v>
+      </c>
+      <c r="C4745" t="n">
+        <v>805661</v>
+      </c>
+      <c r="D4745" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4745" t="n">
+        <v>805661</v>
+      </c>
+    </row>
+    <row r="4746">
+      <c r="A4746" s="2" t="n">
+        <v>45427</v>
+      </c>
+      <c r="B4746" t="n">
+        <v>805661</v>
+      </c>
+      <c r="C4746" t="n">
+        <v>706108</v>
+      </c>
+      <c r="D4746" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4746" t="n">
+        <v>706108</v>
+      </c>
+    </row>
+    <row r="4747">
+      <c r="A4747" s="2" t="n">
+        <v>45428</v>
+      </c>
+      <c r="B4747" t="n">
+        <v>706108</v>
+      </c>
+      <c r="C4747" t="n">
+        <v>716876</v>
+      </c>
+      <c r="D4747" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4747" t="n">
+        <v>716876</v>
+      </c>
+    </row>
+    <row r="4748">
+      <c r="A4748" s="2" t="n">
+        <v>45429</v>
+      </c>
+      <c r="B4748" t="n">
+        <v>716876</v>
+      </c>
+      <c r="C4748" t="n">
+        <v>724577</v>
+      </c>
+      <c r="D4748" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4748" t="n">
+        <v>724577</v>
+      </c>
+    </row>
+    <row r="4749">
+      <c r="A4749" s="2" t="n">
+        <v>45432</v>
+      </c>
+      <c r="B4749" t="n">
+        <v>724577</v>
+      </c>
+      <c r="C4749" t="n">
+        <v>737727</v>
+      </c>
+      <c r="D4749" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4749" t="n">
+        <v>737727</v>
+      </c>
+    </row>
+    <row r="4750">
+      <c r="A4750" s="2" t="n">
+        <v>45433</v>
+      </c>
+      <c r="B4750" t="n">
+        <v>737727</v>
+      </c>
+      <c r="C4750" t="n">
+        <v>738412</v>
+      </c>
+      <c r="D4750" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4750" t="n">
+        <v>738412</v>
+      </c>
+    </row>
+    <row r="4751">
+      <c r="A4751" s="2" t="n">
+        <v>45433</v>
+      </c>
+      <c r="B4751" t="n">
+        <v>737727</v>
+      </c>
+      <c r="C4751" t="n">
+        <v>738412</v>
+      </c>
+      <c r="D4751" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4751" t="n">
+        <v>738412</v>
+      </c>
+    </row>
+    <row r="4752">
+      <c r="A4752" s="2" t="n">
+        <v>45434</v>
+      </c>
+      <c r="B4752" t="n">
+        <v>738412</v>
+      </c>
+      <c r="C4752" t="n">
+        <v>710882</v>
+      </c>
+      <c r="D4752" t="n">
+        <v>962428</v>
+      </c>
+      <c r="E4752" t="n">
+        <v>710882</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>